<commit_message>
Create a new function for extraction of network from txt file also, changed the order of the code lines in main file
</commit_message>
<xml_diff>
--- a/Thesis code/Solutions/solutionsFullWithMotifs.xlsx
+++ b/Thesis code/Solutions/solutionsFullWithMotifs.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Motif #3</t>
+          <t>Motif #4</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -560,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -737,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
         <v>1</v>
@@ -882,7 +882,7 @@
         <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1053,10 +1053,10 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
         <v>1</v>
@@ -1233,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" t="n">
         <v>1</v>
@@ -1285,7 +1285,7 @@
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" t="n">
         <v>1</v>
@@ -1578,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="G39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -1662,7 +1662,7 @@
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" t="n">
         <v>1</v>
@@ -2361,7 +2361,7 @@
         <v>1</v>
       </c>
       <c r="G66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H66" t="n">
         <v>1</v>
@@ -2419,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H68" t="n">
         <v>1</v>
@@ -2572,7 +2572,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Motif #3</t>
+          <t>Motif #4</t>
         </is>
       </c>
     </row>
@@ -2738,7 +2738,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
@@ -2773,7 +2773,7 @@
         <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
@@ -3144,7 +3144,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
@@ -3582,7 +3582,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" t="n">
         <v>1</v>
@@ -3608,10 +3608,10 @@
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" t="n">
         <v>1</v>
@@ -3933,7 +3933,7 @@
         <v>1</v>
       </c>
       <c r="H48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48" t="n">
         <v>1</v>
@@ -3985,13 +3985,13 @@
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50" t="n">
         <v>1</v>
       </c>
       <c r="H50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" t="n">
         <v>1</v>
@@ -4078,7 +4078,7 @@
         <v>1</v>
       </c>
       <c r="H53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" t="n">
         <v>1</v>
@@ -4133,7 +4133,7 @@
         <v>1</v>
       </c>
       <c r="G55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -4481,7 +4481,7 @@
         <v>1</v>
       </c>
       <c r="G67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67" t="n">
         <v>1</v>
@@ -4663,7 +4663,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Motif #3</t>
+          <t>Motif #4</t>
         </is>
       </c>
     </row>
@@ -4887,7 +4887,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -5467,7 +5467,7 @@
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" t="n">
         <v>1</v>
@@ -5496,13 +5496,13 @@
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30" t="n">
         <v>1</v>
       </c>
       <c r="H30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" t="n">
         <v>1</v>
@@ -5525,7 +5525,7 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
@@ -5560,7 +5560,7 @@
         <v>1</v>
       </c>
       <c r="H32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" t="n">
         <v>1</v>
@@ -5786,13 +5786,13 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" t="n">
         <v>1</v>
       </c>
       <c r="H40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" t="n">
         <v>1</v>
@@ -6134,13 +6134,13 @@
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52" t="n">
         <v>1</v>
       </c>
       <c r="H52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52" t="n">
         <v>1</v>
@@ -6192,7 +6192,7 @@
         <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54" t="n">
         <v>1</v>
@@ -6343,7 +6343,7 @@
         <v>1</v>
       </c>
       <c r="H59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I59" t="n">
         <v>1</v>
@@ -6482,13 +6482,13 @@
         <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" t="n">
         <v>1</v>
       </c>
       <c r="H64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64" t="n">
         <v>1</v>
@@ -6627,13 +6627,13 @@
         <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69" t="n">
         <v>1</v>
       </c>
       <c r="H69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69" t="n">
         <v>1</v>
@@ -6754,7 +6754,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Motif #3</t>
+          <t>Motif #4</t>
         </is>
       </c>
     </row>
@@ -6781,7 +6781,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
@@ -7239,13 +7239,13 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" t="n">
         <v>1</v>
@@ -7622,7 +7622,7 @@
         <v>1</v>
       </c>
       <c r="H31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" t="n">
         <v>1</v>
@@ -7674,7 +7674,7 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" t="n">
         <v>1</v>
@@ -7877,7 +7877,7 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" t="n">
         <v>1</v>
@@ -8080,10 +8080,10 @@
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -8489,10 +8489,10 @@
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" t="n">
         <v>1</v>
@@ -8845,7 +8845,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Motif #3</t>
+          <t>Motif #4</t>
         </is>
       </c>
     </row>
@@ -9533,13 +9533,13 @@
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" t="n">
         <v>1</v>
@@ -9623,10 +9623,10 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" t="n">
         <v>1</v>
@@ -9968,7 +9968,7 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" t="n">
         <v>1</v>
@@ -10026,13 +10026,13 @@
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" t="n">
         <v>1</v>
       </c>
       <c r="H42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" t="n">
         <v>1</v>
@@ -10606,10 +10606,10 @@
         <v>0</v>
       </c>
       <c r="F62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -10754,10 +10754,10 @@
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67" t="n">
         <v>1</v>
@@ -10936,7 +10936,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Motif #3</t>
+          <t>Motif #4</t>
         </is>
       </c>
     </row>
@@ -11044,7 +11044,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
         <v>1</v>
@@ -11250,7 +11250,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
         <v>1</v>
@@ -11311,7 +11311,7 @@
         <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" t="n">
         <v>1</v>
@@ -11421,13 +11421,13 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
         <v>1</v>
       </c>
       <c r="H18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" t="n">
         <v>1</v>
@@ -11485,7 +11485,7 @@
         <v>1</v>
       </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="n">
         <v>1</v>
@@ -11946,7 +11946,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" t="n">
         <v>1</v>
@@ -12123,7 +12123,7 @@
         <v>1</v>
       </c>
       <c r="H42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" t="n">
         <v>1</v>
@@ -12700,7 +12700,7 @@
         <v>1</v>
       </c>
       <c r="G62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -12732,7 +12732,7 @@
         <v>1</v>
       </c>
       <c r="H63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I63" t="n">
         <v>1</v>
@@ -12964,7 +12964,7 @@
         <v>1</v>
       </c>
       <c r="H71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I71" t="n">
         <v>1</v>
@@ -13027,7 +13027,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Motif #3</t>
+          <t>Motif #4</t>
         </is>
       </c>
     </row>
@@ -13170,7 +13170,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
@@ -13309,13 +13309,13 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
@@ -13370,7 +13370,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
@@ -13657,10 +13657,10 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -13889,7 +13889,7 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
         <v>1</v>
@@ -14095,10 +14095,10 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38" t="n">
         <v>1</v>
@@ -14266,7 +14266,7 @@
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" t="n">
         <v>1</v>
@@ -14414,10 +14414,10 @@
         <v>1</v>
       </c>
       <c r="G49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" t="n">
         <v>1</v>
@@ -14446,7 +14446,7 @@
         <v>1</v>
       </c>
       <c r="H50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" t="n">
         <v>1</v>
@@ -14469,13 +14469,13 @@
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51" t="n">
         <v>1</v>
       </c>
       <c r="H51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" t="n">
         <v>1</v>
@@ -14530,7 +14530,7 @@
         <v>1</v>
       </c>
       <c r="G53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -14617,7 +14617,7 @@
         <v>1</v>
       </c>
       <c r="G56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56" t="n">
         <v>1</v>
@@ -14849,7 +14849,7 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64" t="n">
         <v>1</v>
@@ -14875,7 +14875,7 @@
         <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65" t="n">
         <v>0</v>
@@ -15118,7 +15118,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Motif #3</t>
+          <t>Motif #4</t>
         </is>
       </c>
     </row>
@@ -15780,7 +15780,7 @@
         <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
         <v>1</v>
@@ -16618,7 +16618,7 @@
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G53" t="n">
         <v>1</v>
@@ -16972,7 +16972,7 @@
         <v>1</v>
       </c>
       <c r="H65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65" t="n">
         <v>1</v>
@@ -16995,13 +16995,13 @@
         <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66" t="n">
         <v>1</v>
       </c>
       <c r="H66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I66" t="n">
         <v>1</v>
@@ -17209,7 +17209,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Motif #3</t>
+          <t>Motif #4</t>
         </is>
       </c>
     </row>
@@ -17262,7 +17262,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
@@ -17468,7 +17468,7 @@
         <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
@@ -17868,10 +17868,10 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -17984,13 +17984,13 @@
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" t="n">
         <v>1</v>
@@ -18132,7 +18132,7 @@
         <v>1</v>
       </c>
       <c r="G33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -18422,7 +18422,7 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" t="n">
         <v>1</v>
@@ -18570,7 +18570,7 @@
         <v>1</v>
       </c>
       <c r="H48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48" t="n">
         <v>1</v>
@@ -18596,7 +18596,7 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" t="n">
         <v>1</v>
@@ -18654,7 +18654,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51" t="n">
         <v>1</v>
@@ -18683,10 +18683,10 @@
         <v>1</v>
       </c>
       <c r="G52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52" t="n">
         <v>1</v>
@@ -18709,10 +18709,10 @@
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -18889,7 +18889,7 @@
         <v>1</v>
       </c>
       <c r="H59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I59" t="n">
         <v>1</v>
@@ -19144,7 +19144,7 @@
         <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68" t="n">
         <v>1</v>
@@ -19202,7 +19202,7 @@
         <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G70" t="n">
         <v>0</v>
@@ -19231,13 +19231,13 @@
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G71" t="n">
         <v>1</v>
       </c>
       <c r="H71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I71" t="n">
         <v>1</v>
@@ -19300,7 +19300,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Motif #3</t>
+          <t>Motif #4</t>
         </is>
       </c>
     </row>
@@ -19382,10 +19382,10 @@
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
@@ -19469,7 +19469,7 @@
         <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
         <v>1</v>
@@ -19585,10 +19585,10 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
@@ -19701,7 +19701,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
         <v>1</v>
@@ -19843,13 +19843,13 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="n">
         <v>1</v>
@@ -20078,7 +20078,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
         <v>1</v>
@@ -20278,7 +20278,7 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
@@ -20368,7 +20368,7 @@
         <v>1</v>
       </c>
       <c r="G38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -20487,7 +20487,7 @@
         <v>0</v>
       </c>
       <c r="H42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" t="n">
         <v>1</v>
@@ -21032,10 +21032,10 @@
         <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61" t="n">
         <v>1</v>
@@ -21090,7 +21090,7 @@
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G63" t="n">
         <v>1</v>
@@ -21296,7 +21296,7 @@
         <v>1</v>
       </c>
       <c r="G70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H70" t="n">
         <v>0</v>
@@ -21391,7 +21391,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Motif #3</t>
+          <t>Motif #4</t>
         </is>
       </c>
     </row>
@@ -21766,7 +21766,7 @@
         <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" t="n">
         <v>1</v>
@@ -22259,7 +22259,7 @@
         <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" t="n">
         <v>1</v>
@@ -22288,7 +22288,7 @@
         <v>1</v>
       </c>
       <c r="H32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" t="n">
         <v>1</v>
@@ -22311,7 +22311,7 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" t="n">
         <v>1</v>
@@ -22372,10 +22372,10 @@
         <v>1</v>
       </c>
       <c r="G35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" t="n">
         <v>1</v>
@@ -22926,7 +22926,7 @@
         <v>1</v>
       </c>
       <c r="H54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" t="n">
         <v>1</v>
@@ -23039,7 +23039,7 @@
         <v>1</v>
       </c>
       <c r="G58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H58" t="n">
         <v>1</v>
@@ -23187,7 +23187,7 @@
         <v>1</v>
       </c>
       <c r="H63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I63" t="n">
         <v>1</v>

</xml_diff>